<commit_message>
Added main.py and updated search query
</commit_message>
<xml_diff>
--- a/DATA/Protest-Query.xlsx
+++ b/DATA/Protest-Query.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2022\Sem 1\ELEN4002 Capstone Project\Code\Team-Riot\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668ADDE8-0AA1-403E-99B6-FA174AE0C9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891CCC06-C564-4297-920F-992F64511E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{C53576D5-AA90-456F-BE37-26B46836C21A}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C53576D5-AA90-456F-BE37-26B46836C21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>University</t>
   </si>
@@ -131,9 +131,6 @@
     <t>burning</t>
   </si>
   <si>
-    <t>fees</t>
-  </si>
-  <si>
     <t>must fall</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>picket</t>
   </si>
   <si>
-    <t>gather</t>
-  </si>
-  <si>
     <t>dance</t>
   </si>
   <si>
@@ -222,6 +216,18 @@
   </si>
   <si>
     <t>amandla</t>
+  </si>
+  <si>
+    <t>gathering</t>
+  </si>
+  <si>
+    <t>mass%meeting</t>
+  </si>
+  <si>
+    <t>free%education</t>
+  </si>
+  <si>
+    <t>fee</t>
   </si>
 </sst>
 </file>
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B80DAE-5665-4A1A-90FE-B069781CF2D5}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +627,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +655,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,12 +669,12 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -677,12 +683,12 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -690,13 +696,10 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -704,13 +707,10 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -718,40 +718,49 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,7 +776,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,66 +784,71 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>